<commit_message>
Update pairwise comparisons and fix bugs
</commit_message>
<xml_diff>
--- a/data/dims-coefficients.xlsx
+++ b/data/dims-coefficients.xlsx
@@ -273,7 +273,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,12 +284,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -347,13 +341,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -370,7 +361,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -379,7 +370,7 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -705,16 +696,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="5.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="35.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="135.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="14.147857142857141" customWidth="1" bestFit="1" hidden="1"/>
-    <col min="6" max="6" style="14" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="5.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="35.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="135.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="6" max="6" style="13" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -727,359 +718,359 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="7">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>0.22935577168462573</v>
       </c>
-      <c r="F2" s="10">
-        <v>0.04409100048181188</v>
-      </c>
-      <c r="G2" s="7">
+      <c r="F2" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G2" s="6">
         <v>0</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <f>F2*G2</f>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>0.9774572303085642</v>
       </c>
-      <c r="F3" s="10">
-        <v>0.18790487327149444</v>
-      </c>
-      <c r="G3" s="7">
+      <c r="F3" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G3" s="6">
         <v>3</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <f>F3*G3</f>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>0.21263528824509892</v>
       </c>
-      <c r="F4" s="10">
-        <v>0.04087668048465908</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="6">
         <v>4</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <f>F4*G4</f>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="4"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>0.6653837744358718</v>
       </c>
-      <c r="F5" s="10">
-        <v>0.12791235251573305</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="6">
         <v>0</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <f>F5*G5</f>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="4"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>0.4489660074714332</v>
       </c>
-      <c r="F6" s="10">
-        <v>0.08630853414475921</v>
-      </c>
-      <c r="G6" s="7">
+      <c r="F6" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="6">
         <v>1</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="9">
         <f>F6*G6</f>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="4"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>0.8388025565934849</v>
       </c>
-      <c r="F7" s="10">
-        <v>0.16125011223943608</v>
-      </c>
-      <c r="G7" s="7">
+      <c r="F7" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="G7" s="6">
         <v>1</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="9">
         <f>F7*G7</f>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="4"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>0.5722210763953692</v>
       </c>
-      <c r="F8" s="10">
-        <v>0.11000289885768919</v>
-      </c>
-      <c r="G8" s="7">
+      <c r="F8" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="G8" s="6">
         <v>0</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <f>F8*G8</f>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="4"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>0.029385463970410752</v>
       </c>
-      <c r="F9" s="10">
-        <v>0.005649016358128543</v>
-      </c>
-      <c r="G9" s="7">
+      <c r="F9" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="6">
         <v>1</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="9">
         <f>F9*G9</f>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>0.04508257384198999</v>
       </c>
-      <c r="F10" s="10">
-        <v>0.008666604595945048</v>
-      </c>
-      <c r="G10" s="7">
+      <c r="F10" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="G10" s="6">
         <v>4</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <f>F10*G10</f>
       </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="4"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>0.345033234967395</v>
       </c>
-      <c r="F11" s="10">
-        <v>0.06632865795113661</v>
-      </c>
-      <c r="G11" s="7">
+      <c r="F11" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="G11" s="6">
         <v>2</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="9">
         <f>F11*G11</f>
       </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="4"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>0.7532668865786963</v>
       </c>
-      <c r="F12" s="10">
-        <v>0.14480686670812276</v>
-      </c>
-      <c r="G12" s="7">
+      <c r="F12" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="G12" s="6">
         <v>1</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="9">
         <f>F12*G12</f>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="4"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="10">
+      <c r="E13" s="9">
         <v>0.08428283465885222</v>
       </c>
-      <c r="F13" s="10">
-        <v>0.016202402391084125</v>
-      </c>
-      <c r="G13" s="7">
+      <c r="F13" s="9">
+        <v>0.33</v>
+      </c>
+      <c r="G13" s="6">
         <v>0</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <f>F13*G13</f>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <f>SUM(H2:H13)</f>
       </c>
     </row>
@@ -1087,160 +1078,160 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>0.42107300433980077</v>
       </c>
-      <c r="F14" s="4">
-        <v>0.10595684007792218</v>
+      <c r="F14" s="3">
+        <v>0.5</v>
       </c>
       <c r="G14" s="1">
         <v>3</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f>F14*G14</f>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="4"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.14857812045298568</v>
       </c>
-      <c r="F15" s="4">
-        <v>0.0373875028454946</v>
+      <c r="F15" s="3">
+        <v>0.5</v>
       </c>
       <c r="G15" s="1">
         <v>3</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f>F15*G15</f>
       </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="4"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>0.1957216079891657</v>
       </c>
-      <c r="F16" s="4">
-        <v>0.04925046940498341</v>
+      <c r="F16" s="3">
+        <v>0.5</v>
       </c>
       <c r="G16" s="1">
         <v>2</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f>F16*G16</f>
       </c>
-      <c r="I16" s="6"/>
-      <c r="J16" s="4"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>0.8215948180489099</v>
       </c>
-      <c r="F17" s="4">
-        <v>0.20674227473059928</v>
+      <c r="F17" s="3">
+        <v>0.5</v>
       </c>
       <c r="G17" s="1">
         <v>3</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <f>F17*G17</f>
       </c>
-      <c r="I17" s="6"/>
-      <c r="J17" s="4"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>0.7189042007720691</v>
       </c>
-      <c r="F18" s="4">
-        <v>0.18090168841857657</v>
+      <c r="F18" s="3">
+        <v>0.5</v>
       </c>
       <c r="G18" s="1">
         <v>3</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <f>F18*G18</f>
       </c>
-      <c r="I18" s="6"/>
-      <c r="J18" s="4"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>0.17461010351383177</v>
       </c>
-      <c r="F19" s="4">
-        <v>0.04393806922629103</v>
+      <c r="F19" s="3">
+        <v>0.5</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -1248,55 +1239,55 @@
       <c r="H19" s="1">
         <f>F19*G19</f>
       </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>0.0037087720736994623</v>
       </c>
-      <c r="F20" s="4">
-        <v>0.0009332580465816704</v>
+      <c r="F20" s="9">
+        <v>0.25</v>
       </c>
       <c r="G20" s="1">
         <v>3</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f>F20*G20</f>
       </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="4"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>0.3705499153821572</v>
       </c>
-      <c r="F21" s="4">
-        <v>0.09324344643417375</v>
+      <c r="F21" s="9">
+        <v>0.25</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -1304,27 +1295,27 @@
       <c r="H21" s="1">
         <f>F21*G21</f>
       </c>
-      <c r="I21" s="6"/>
-      <c r="J21" s="4"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>0.9171958244724371</v>
       </c>
-      <c r="F22" s="4">
-        <v>0.23079886454876686</v>
+      <c r="F22" s="9">
+        <v>0.25</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
@@ -1332,322 +1323,322 @@
       <c r="H22" s="1">
         <f>F22*G22</f>
       </c>
-      <c r="I22" s="6"/>
-      <c r="J22" s="4"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>0.20206855826356607</v>
       </c>
-      <c r="F23" s="4">
-        <v>0.05084758626661072</v>
+      <c r="F23" s="9">
+        <v>0.25</v>
       </c>
       <c r="G23" s="1">
         <v>2</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <f>F23*G23</f>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="3">
         <f>SUM(H14:H23)</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E24" s="9">
         <v>0.5639378874995834</v>
       </c>
-      <c r="F24" s="10">
-        <v>0.11508475224766167</v>
-      </c>
-      <c r="G24" s="7">
+      <c r="F24" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G24" s="6">
         <v>1</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24" s="9">
         <f>F24*G24</f>
       </c>
-      <c r="I24" s="6"/>
-      <c r="J24" s="4"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="9">
         <v>0.3829923073236283</v>
       </c>
-      <c r="F25" s="10">
-        <v>0.07815856281004462</v>
-      </c>
-      <c r="G25" s="7">
+      <c r="F25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G25" s="6">
         <v>1</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25" s="9">
         <f>F25*G25</f>
       </c>
-      <c r="I25" s="6"/>
-      <c r="J25" s="4"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
-      <c r="A26" s="7">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E26" s="9">
         <v>0.8915943921104035</v>
       </c>
-      <c r="F26" s="10">
-        <v>0.18195074669727007</v>
-      </c>
-      <c r="G26" s="7">
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6">
         <v>3</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26" s="9">
         <f>F26*G26</f>
       </c>
-      <c r="I26" s="6"/>
-      <c r="J26" s="4"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
-      <c r="A27" s="7">
+      <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="9">
         <v>0.7949834429117825</v>
       </c>
-      <c r="F27" s="10">
-        <v>0.16223501665077106</v>
-      </c>
-      <c r="G27" s="7">
+      <c r="F27" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="6">
         <v>0</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="6">
         <f>F27*G27</f>
       </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="4"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>27</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="9">
         <v>0.7941342429121413</v>
       </c>
-      <c r="F28" s="10">
-        <v>0.16206171747415296</v>
-      </c>
-      <c r="G28" s="7">
+      <c r="F28" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G28" s="6">
         <v>0</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="6">
         <f>F28*G28</f>
       </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="4"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>28</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C29" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="9">
         <v>0.3597161637183648</v>
       </c>
-      <c r="F29" s="10">
-        <v>0.07340851980092913</v>
-      </c>
-      <c r="G29" s="7">
+      <c r="F29" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G29" s="6">
         <v>1</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29" s="9">
         <f>F29*G29</f>
       </c>
-      <c r="I29" s="6"/>
-      <c r="J29" s="4"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>29</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="9">
         <v>0.037293358772855334</v>
       </c>
-      <c r="F30" s="10">
-        <v>0.007610584516473698</v>
-      </c>
-      <c r="G30" s="7">
+      <c r="F30" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G30" s="6">
         <v>2</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30" s="9">
         <f>F30*G30</f>
       </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="4"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>30</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="9">
         <v>0.546744657473765</v>
       </c>
-      <c r="F31" s="10">
-        <v>0.11157607041989596</v>
-      </c>
-      <c r="G31" s="7">
+      <c r="F31" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G31" s="6">
         <v>1</v>
       </c>
-      <c r="H31" s="10">
+      <c r="H31" s="9">
         <f>F31*G31</f>
       </c>
-      <c r="I31" s="6"/>
-      <c r="J31" s="4"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>31</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="9">
         <v>0.3549741449250039</v>
       </c>
-      <c r="F32" s="10">
-        <v>0.07244079964932272</v>
-      </c>
-      <c r="G32" s="7">
+      <c r="F32" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G32" s="6">
         <v>4</v>
       </c>
-      <c r="H32" s="10">
+      <c r="H32" s="9">
         <f>F32*G32</f>
       </c>
-      <c r="I32" s="6"/>
-      <c r="J32" s="4"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>32</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="9">
         <v>0.1738257922790245</v>
       </c>
-      <c r="F33" s="10">
-        <v>0.03547322973347807</v>
-      </c>
-      <c r="G33" s="7">
+      <c r="F33" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G33" s="6">
         <v>3</v>
       </c>
-      <c r="H33" s="10">
+      <c r="H33" s="9">
         <f>F33*G33</f>
       </c>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="3">
         <f>SUM(H24:H33)</f>
       </c>
     </row>
@@ -1655,20 +1646,20 @@
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>0.20416608369861822</v>
       </c>
-      <c r="F34" s="4">
-        <v>0.0437084584476013</v>
+      <c r="F34" s="3">
+        <v>0.5</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
@@ -1676,223 +1667,223 @@
       <c r="H34" s="1">
         <f>F34*G34</f>
       </c>
-      <c r="I34" s="6"/>
-      <c r="J34" s="4"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="11" t="s">
+      <c r="D35" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>0.9876063558060288</v>
       </c>
-      <c r="F35" s="4">
-        <v>0.2114295899854541</v>
+      <c r="F35" s="3">
+        <v>0.5</v>
       </c>
       <c r="G35" s="1">
         <v>1</v>
       </c>
-      <c r="H35" s="4">
+      <c r="H35" s="3">
         <f>F35*G35</f>
       </c>
-      <c r="I35" s="6"/>
-      <c r="J35" s="4"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="11" t="s">
+      <c r="D36" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>0.12293693103907422</v>
       </c>
-      <c r="F36" s="4">
-        <v>0.02631868939568325</v>
+      <c r="F36" s="3">
+        <v>1</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="3">
         <f>F36*G36</f>
       </c>
-      <c r="I36" s="6"/>
-      <c r="J36" s="4"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>0.9521987525747528</v>
       </c>
-      <c r="F37" s="4">
-        <v>0.203849429135389</v>
+      <c r="F37" s="3">
+        <v>0.5</v>
       </c>
       <c r="G37" s="1">
         <v>1</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f>F37*G37</f>
       </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="4"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>0.642370787678666</v>
       </c>
-      <c r="F38" s="4">
-        <v>0.13752057331251985</v>
+      <c r="F38" s="3">
+        <v>0.5</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
       </c>
-      <c r="H38" s="4">
+      <c r="H38" s="3">
         <f>F38*G38</f>
       </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="4"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="20.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E39" s="4">
+      <c r="E39" s="3">
         <v>0.3123072636522166</v>
       </c>
-      <c r="F39" s="4">
-        <v>0.06685963118329315</v>
+      <c r="F39" s="9">
+        <v>0.2</v>
       </c>
       <c r="G39" s="1">
         <v>4</v>
       </c>
-      <c r="H39" s="4">
+      <c r="H39" s="3">
         <f>F39*G39</f>
       </c>
-      <c r="I39" s="6"/>
-      <c r="J39" s="4"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="20.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="4">
+      <c r="E40" s="3">
         <v>0.29412414891305605</v>
       </c>
-      <c r="F40" s="4">
-        <v>0.06296693803550396</v>
+      <c r="F40" s="9">
+        <v>0.2</v>
       </c>
       <c r="G40" s="1">
         <v>4</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f>F40*G40</f>
       </c>
-      <c r="I40" s="6"/>
-      <c r="J40" s="4"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="20.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="11" t="s">
+      <c r="D41" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="4">
+      <c r="E41" s="3">
         <v>0.4810439434160897</v>
       </c>
-      <c r="F41" s="4">
-        <v>0.10298326162395173</v>
+      <c r="F41" s="9">
+        <v>0.2</v>
       </c>
       <c r="G41" s="1">
         <v>2</v>
       </c>
-      <c r="H41" s="4">
+      <c r="H41" s="3">
         <f>F41*G41</f>
       </c>
-      <c r="I41" s="6"/>
-      <c r="J41" s="4"/>
+      <c r="I41" s="5"/>
+      <c r="J41" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>54</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E42" s="4">
+      <c r="E42" s="3">
         <v>0.6743343725835366</v>
       </c>
-      <c r="F42" s="4">
-        <v>0.14436342888060344</v>
+      <c r="F42" s="9">
+        <v>0.2</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
@@ -1900,266 +1891,266 @@
       <c r="H42" s="1">
         <f>F42*G42</f>
       </c>
-      <c r="I42" s="6" t="s">
+      <c r="I42" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="3">
         <f>SUM(H34:H42)</f>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
-      <c r="A43" s="7">
+      <c r="A43" s="6">
         <v>42</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C43" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="9">
         <v>0.3314614630361977</v>
       </c>
-      <c r="F43" s="10">
-        <v>0.08025657128739001</v>
-      </c>
-      <c r="G43" s="7">
+      <c r="F43" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G43" s="6">
         <v>1</v>
       </c>
-      <c r="H43" s="10">
+      <c r="H43" s="9">
         <f>F43*G43</f>
       </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="4"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
-      <c r="A44" s="7">
+      <c r="A44" s="6">
         <v>43</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="10">
+      <c r="E44" s="9">
         <v>0.03598080991121799</v>
       </c>
-      <c r="F44" s="10">
-        <v>0.008712012579581057</v>
-      </c>
-      <c r="G44" s="7">
+      <c r="F44" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G44" s="6">
         <v>2</v>
       </c>
-      <c r="H44" s="10">
+      <c r="H44" s="9">
         <f>F44*G44</f>
       </c>
-      <c r="I44" s="6"/>
-      <c r="J44" s="4"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <v>44</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="B45" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="9" t="s">
+      <c r="C45" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="9">
         <v>0.6587832433295059</v>
       </c>
-      <c r="F45" s="10">
-        <v>0.1595108035996286</v>
-      </c>
-      <c r="G45" s="7">
+      <c r="F45" s="9">
+        <v>1</v>
+      </c>
+      <c r="G45" s="6">
         <v>2</v>
       </c>
-      <c r="H45" s="10">
+      <c r="H45" s="9">
         <f>F45*G45</f>
       </c>
-      <c r="I45" s="6"/>
-      <c r="J45" s="4"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
-      <c r="A46" s="7">
+      <c r="A46" s="6">
         <v>45</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="B46" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="10">
+      <c r="E46" s="9">
         <v>0.7449981286269592</v>
       </c>
-      <c r="F46" s="10">
-        <v>0.18038596363943565</v>
-      </c>
-      <c r="G46" s="7">
+      <c r="F46" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G46" s="6">
         <v>2</v>
       </c>
-      <c r="H46" s="10">
+      <c r="H46" s="9">
         <f>F46*G46</f>
       </c>
-      <c r="I46" s="6"/>
-      <c r="J46" s="4"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
-      <c r="A47" s="7">
+      <c r="A47" s="6">
         <v>46</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C47" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="10">
+      <c r="E47" s="9">
         <v>0.23777100145271024</v>
       </c>
-      <c r="F47" s="10">
-        <v>0.05757135430878009</v>
-      </c>
-      <c r="G47" s="7">
+      <c r="F47" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G47" s="6">
         <v>4</v>
       </c>
-      <c r="H47" s="10">
+      <c r="H47" s="9">
         <f>F47*G47</f>
       </c>
-      <c r="I47" s="6"/>
-      <c r="J47" s="4"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
-      <c r="A48" s="7">
+      <c r="A48" s="6">
         <v>47</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="9">
         <v>0.7460047460721294</v>
       </c>
-      <c r="F48" s="10">
-        <v>0.18062969533604803</v>
-      </c>
-      <c r="G48" s="7">
+      <c r="F48" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G48" s="6">
         <v>1</v>
       </c>
-      <c r="H48" s="10">
+      <c r="H48" s="9">
         <f>F48*G48</f>
       </c>
-      <c r="I48" s="6"/>
-      <c r="J48" s="4"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
-      <c r="A49" s="7">
+      <c r="A49" s="6">
         <v>48</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C49" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="9">
         <v>0.11599250894447277</v>
       </c>
-      <c r="F49" s="10">
-        <v>0.028085198736628646</v>
-      </c>
-      <c r="G49" s="7">
+      <c r="F49" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G49" s="6">
         <v>1</v>
       </c>
-      <c r="H49" s="10">
+      <c r="H49" s="9">
         <f>F49*G49</f>
       </c>
-      <c r="I49" s="6"/>
-      <c r="J49" s="4"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
-      <c r="A50" s="7">
+      <c r="A50" s="6">
         <v>49</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="9" t="s">
+      <c r="C50" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="8" t="s">
+      <c r="D50" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="10">
+      <c r="E50" s="9">
         <v>0.6406476871314409</v>
       </c>
-      <c r="F50" s="10">
-        <v>0.15511965192391325</v>
-      </c>
-      <c r="G50" s="7">
+      <c r="F50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G50" s="6">
         <v>1</v>
       </c>
-      <c r="H50" s="10">
+      <c r="H50" s="9">
         <f>F50*G50</f>
       </c>
-      <c r="I50" s="6"/>
-      <c r="J50" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="7">
+      <c r="I50" s="5"/>
+      <c r="J50" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
+      <c r="A51" s="6">
         <v>50</v>
       </c>
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="9" t="s">
+      <c r="C51" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="8" t="s">
+      <c r="D51" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="9">
         <v>0.6183831338624901</v>
       </c>
-      <c r="F51" s="10">
-        <v>0.14972874858859456</v>
-      </c>
-      <c r="G51" s="7">
+      <c r="F51" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G51" s="6">
         <v>3</v>
       </c>
-      <c r="H51" s="10">
+      <c r="H51" s="9">
         <f>F51*G51</f>
       </c>
-      <c r="I51" s="6" t="s">
+      <c r="I51" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="3">
         <f>SUM(H43:H51)</f>
       </c>
     </row>

</xml_diff>

<commit_message>
Update default weights to sum up one
</commit_message>
<xml_diff>
--- a/data/dims-coefficients.xlsx
+++ b/data/dims-coefficients.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leonr\Desktop\digital_awareness\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5359B-B7FE-4693-8F00-C8E36A8D40A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Answer"/>
+    <sheet name="Answer" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -271,8 +290,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -303,7 +321,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -324,16 +342,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -341,62 +359,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -407,10 +422,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -448,71 +463,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -540,7 +555,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -563,11 +578,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -576,13 +591,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -592,7 +607,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -601,7 +616,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -610,7 +625,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -618,10 +633,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -686,29 +701,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="5.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="35.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="135.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="13" width="14.147857142857141" customWidth="1" bestFit="1" hidden="1"/>
-    <col min="6" max="6" style="13" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="5" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="135.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="12" hidden="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -731,1427 +748,1436 @@
       <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5"/>
       <c r="J1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>0.22935577168462573</v>
       </c>
-      <c r="F2" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
-        <f>F2*G2</f>
-      </c>
-      <c r="I2" s="5"/>
+      <c r="F2" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5">
+        <f t="shared" ref="H2:H33" si="0">F2*G2</f>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J2" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="9">
-        <v>0.9774572303085642</v>
-      </c>
-      <c r="F3" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G3" s="6">
+      <c r="E3" s="8">
+        <v>0.97745723030856424</v>
+      </c>
+      <c r="F3" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="H3" s="9">
-        <f>F3*G3</f>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>0.21263528824509892</v>
       </c>
-      <c r="F4" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="F4" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G4" s="5">
+        <v>2</v>
+      </c>
+      <c r="H4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="H4" s="9">
-        <f>F4*G4</f>
-      </c>
-      <c r="I4" s="5"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="9">
-        <v>0.6653837744358718</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <f>F5*G5</f>
-      </c>
-      <c r="I5" s="5"/>
+      <c r="E5" s="8">
+        <v>0.66538377443587182</v>
+      </c>
+      <c r="F5" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G5" s="5">
+        <v>2</v>
+      </c>
+      <c r="H5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J5" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9">
-        <v>0.4489660074714332</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9">
-        <f>F6*G6</f>
-      </c>
-      <c r="I6" s="5"/>
+      <c r="E6" s="8">
+        <v>0.44896600747143323</v>
+      </c>
+      <c r="F6" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G6" s="5">
+        <v>2</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J6" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>0.8388025565934849</v>
       </c>
-      <c r="F7" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9">
-        <f>F7*G7</f>
-      </c>
-      <c r="I7" s="5"/>
+      <c r="F7" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J7" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="9">
-        <v>0.5722210763953692</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <f>F8*G8</f>
-      </c>
-      <c r="I8" s="5"/>
+      <c r="E8" s="8">
+        <v>0.57222107639536923</v>
+      </c>
+      <c r="F8" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J8" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
-      <c r="A9" s="6">
+    <row r="9" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="9">
-        <v>0.029385463970410752</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="9">
-        <f>F9*G9</f>
-      </c>
-      <c r="I9" s="5"/>
+      <c r="E9" s="8">
+        <v>2.9385463970410752E-2</v>
+      </c>
+      <c r="F9" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G9" s="5">
+        <v>2</v>
+      </c>
+      <c r="H9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J9" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
-      <c r="A10" s="6">
+    <row r="10" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="9">
-        <v>0.04508257384198999</v>
-      </c>
-      <c r="F10" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G10" s="6">
-        <v>4</v>
-      </c>
-      <c r="H10" s="9">
-        <f>F10*G10</f>
-      </c>
-      <c r="I10" s="5"/>
+      <c r="E10" s="8">
+        <v>4.5082573841989992E-2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J10" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
-      <c r="A11" s="6">
+    <row r="11" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="9">
-        <v>0.345033234967395</v>
-      </c>
-      <c r="F11" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="G11" s="6">
-        <v>2</v>
-      </c>
-      <c r="H11" s="9">
-        <f>F11*G11</f>
-      </c>
-      <c r="I11" s="5"/>
+      <c r="E11" s="8">
+        <v>0.34503323496739502</v>
+      </c>
+      <c r="F11" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.25">
-      <c r="A12" s="6">
+    <row r="12" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="9">
-        <v>0.7532668865786963</v>
-      </c>
-      <c r="F12" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="9">
-        <f>F12*G12</f>
-      </c>
-      <c r="I12" s="5"/>
+      <c r="E12" s="8">
+        <v>0.75326688657869634</v>
+      </c>
+      <c r="F12" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>2</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
       <c r="J12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
-      <c r="A13" s="6">
+    <row r="13" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="9">
-        <v>0.08428283465885222</v>
-      </c>
-      <c r="F13" s="9">
-        <v>0.33</v>
-      </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
-        <f>F13*G13</f>
-      </c>
-      <c r="I13" s="5" t="s">
+      <c r="E13" s="8">
+        <v>8.4282834658852224E-2</v>
+      </c>
+      <c r="F13" s="8">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="I13" t="s">
         <v>23</v>
       </c>
       <c r="J13" s="3">
         <f>SUM(H2:H13)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="20.25">
+        <v>1.9919999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="E14" s="3">
         <v>0.42107300433980077</v>
       </c>
       <c r="F14" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G14" s="1">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
       </c>
       <c r="H14" s="3">
-        <f>F14*G14</f>
-      </c>
-      <c r="I14" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="20.25">
+    <row r="15" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="3">
         <v>0.14857812045298568</v>
       </c>
       <c r="F15" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G15" s="1">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
       </c>
       <c r="H15" s="3">
-        <f>F15*G15</f>
-      </c>
-      <c r="I15" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J15" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+    <row r="16" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="3">
-        <v>0.1957216079891657</v>
+        <v>0.19572160798916571</v>
       </c>
       <c r="F16" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="5">
         <v>2</v>
       </c>
       <c r="H16" s="3">
-        <f>F16*G16</f>
-      </c>
-      <c r="I16" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J16" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
+    <row r="17" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="3">
-        <v>0.8215948180489099</v>
+        <v>0.82159481804890988</v>
       </c>
       <c r="F17" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="1">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>2</v>
       </c>
       <c r="H17" s="3">
-        <f>F17*G17</f>
-      </c>
-      <c r="I17" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J17" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25">
+    <row r="18" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>32</v>
       </c>
       <c r="E18" s="3">
-        <v>0.7189042007720691</v>
+        <v>0.71890420077206907</v>
       </c>
       <c r="F18" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G18" s="1">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="5">
+        <v>2</v>
       </c>
       <c r="H18" s="3">
-        <f>F18*G18</f>
-      </c>
-      <c r="I18" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J18" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
+    <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E19" s="3">
         <v>0.17461010351383177</v>
       </c>
       <c r="F19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="5">
+        <v>2</v>
       </c>
       <c r="H19" s="1">
-        <f>F19*G19</f>
-      </c>
-      <c r="I19" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J19" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="20.25">
+    <row r="20" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="9" t="s">
         <v>35</v>
       </c>
       <c r="E20" s="3">
-        <v>0.0037087720736994623</v>
-      </c>
-      <c r="F20" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G20" s="1">
-        <v>3</v>
+        <v>3.7087720736994623E-3</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
       </c>
       <c r="H20" s="3">
-        <f>F20*G20</f>
-      </c>
-      <c r="I20" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J20" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25">
+    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E21" s="3">
         <v>0.3705499153821572</v>
       </c>
-      <c r="F21" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0</v>
+      <c r="F21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
       </c>
       <c r="H21" s="1">
-        <f>F21*G21</f>
-      </c>
-      <c r="I21" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J21" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25">
+    <row r="22" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="9" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="3">
-        <v>0.9171958244724371</v>
-      </c>
-      <c r="F22" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G22" s="1">
-        <v>0</v>
+        <v>0.91719582447243708</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>2</v>
       </c>
       <c r="H22" s="1">
-        <f>F22*G22</f>
-      </c>
-      <c r="I22" s="5"/>
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J22" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="20.25">
+    <row r="23" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E23" s="3">
         <v>0.20206855826356607</v>
       </c>
-      <c r="F23" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="G23" s="1">
+      <c r="F23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G23" s="5">
         <v>2</v>
       </c>
       <c r="H23" s="3">
-        <f>F23*G23</f>
-      </c>
-      <c r="I23" s="5" t="s">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I23" t="s">
         <v>23</v>
       </c>
       <c r="J23" s="3">
         <f>SUM(H14:H23)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="20.25">
-      <c r="A24" s="6">
+        <v>1.9999999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>0.5639378874995834</v>
       </c>
       <c r="F24" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" s="9">
-        <f>F24*G24</f>
-      </c>
-      <c r="I24" s="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="G24" s="5">
+        <v>2</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J24" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="20.25">
-      <c r="A25" s="6">
+    <row r="25" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="9">
-        <v>0.3829923073236283</v>
+      <c r="E25" s="8">
+        <v>0.38299230732362832</v>
       </c>
       <c r="F25" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1</v>
-      </c>
-      <c r="H25" s="9">
-        <f>F25*G25</f>
-      </c>
-      <c r="I25" s="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="G25" s="5">
+        <v>2</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J25" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="20.25">
-      <c r="A26" s="6">
+    <row r="26" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="9">
-        <v>0.8915943921104035</v>
-      </c>
-      <c r="F26" s="9">
-        <v>1</v>
-      </c>
-      <c r="G26" s="6">
-        <v>3</v>
-      </c>
-      <c r="H26" s="9">
-        <f>F26*G26</f>
-      </c>
-      <c r="I26" s="5"/>
+      <c r="E26" s="8">
+        <v>0.89159439211040348</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G26" s="5">
+        <v>2</v>
+      </c>
+      <c r="H26" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J26" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="20.25">
-      <c r="A27" s="6">
+    <row r="27" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="9">
-        <v>0.7949834429117825</v>
-      </c>
-      <c r="F27" s="9">
+      <c r="E27" s="8">
+        <v>0.79498344291178247</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G27" s="5">
+        <v>2</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G27" s="6">
-        <v>0</v>
-      </c>
-      <c r="H27" s="6">
-        <f>F27*G27</f>
-      </c>
-      <c r="I27" s="5"/>
       <c r="J27" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="20.25">
-      <c r="A28" s="6">
+    <row r="28" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>0.7941342429121413</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>2</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G28" s="6">
-        <v>0</v>
-      </c>
-      <c r="H28" s="6">
-        <f>F28*G28</f>
-      </c>
-      <c r="I28" s="5"/>
       <c r="J28" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="20.25">
-      <c r="A29" s="6">
+    <row r="29" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E29" s="9">
-        <v>0.3597161637183648</v>
-      </c>
-      <c r="F29" s="9">
+      <c r="E29" s="8">
+        <v>0.35971616371836479</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G29" s="5">
+        <v>2</v>
+      </c>
+      <c r="H29" s="8">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G29" s="6">
-        <v>1</v>
-      </c>
-      <c r="H29" s="9">
-        <f>F29*G29</f>
-      </c>
-      <c r="I29" s="5"/>
       <c r="J29" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="20.25">
-      <c r="A30" s="6">
+    <row r="30" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="9">
-        <v>0.037293358772855334</v>
-      </c>
-      <c r="F30" s="9">
+      <c r="E30" s="8">
+        <v>3.7293358772855334E-2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G30" s="5">
+        <v>2</v>
+      </c>
+      <c r="H30" s="8">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G30" s="6">
-        <v>2</v>
-      </c>
-      <c r="H30" s="9">
-        <f>F30*G30</f>
-      </c>
-      <c r="I30" s="5"/>
       <c r="J30" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="20.25">
-      <c r="A31" s="6">
+    <row r="31" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="9">
-        <v>0.546744657473765</v>
-      </c>
-      <c r="F31" s="9">
+      <c r="E31" s="8">
+        <v>0.54674465747376499</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G31" s="5">
+        <v>2</v>
+      </c>
+      <c r="H31" s="8">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="G31" s="6">
-        <v>1</v>
-      </c>
-      <c r="H31" s="9">
-        <f>F31*G31</f>
-      </c>
-      <c r="I31" s="5"/>
       <c r="J31" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="20.25">
-      <c r="A32" s="6">
+    <row r="32" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>0.3549741449250039</v>
       </c>
       <c r="F32" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G32" s="6">
-        <v>4</v>
-      </c>
-      <c r="H32" s="9">
-        <f>F32*G32</f>
-      </c>
-      <c r="I32" s="5"/>
+        <v>0.1</v>
+      </c>
+      <c r="G32" s="5">
+        <v>2</v>
+      </c>
+      <c r="H32" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="J32" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="20.25">
-      <c r="A33" s="6">
+    <row r="33" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="9">
+      <c r="E33" s="8">
         <v>0.1738257922790245</v>
       </c>
       <c r="F33" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G33" s="6">
-        <v>3</v>
-      </c>
-      <c r="H33" s="9">
-        <f>F33*G33</f>
-      </c>
-      <c r="I33" s="5" t="s">
+        <v>0.1</v>
+      </c>
+      <c r="G33" s="5">
+        <v>2</v>
+      </c>
+      <c r="H33" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I33" t="s">
         <v>23</v>
       </c>
       <c r="J33" s="3">
         <f>SUM(H24:H33)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="20.25">
+        <v>1.9999999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E34" s="3">
         <v>0.20416608369861822</v>
       </c>
       <c r="F34" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
+        <v>0.11</v>
+      </c>
+      <c r="G34" s="5">
+        <v>2</v>
       </c>
       <c r="H34" s="1">
-        <f>F34*G34</f>
-      </c>
-      <c r="I34" s="5"/>
+        <f t="shared" ref="H34:H65" si="1">F34*G34</f>
+        <v>0.22</v>
+      </c>
       <c r="J34" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="20.25">
+    <row r="35" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="D35" s="9" t="s">
         <v>58</v>
       </c>
       <c r="E35" s="3">
-        <v>0.9876063558060288</v>
+        <v>0.98760635580602885</v>
       </c>
       <c r="F35" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G35" s="1">
-        <v>1</v>
+        <v>0.11</v>
+      </c>
+      <c r="G35" s="5">
+        <v>2</v>
       </c>
       <c r="H35" s="3">
-        <f>F35*G35</f>
-      </c>
-      <c r="I35" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J35" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="20.25">
+    <row r="36" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="B36" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E36" s="3">
         <v>0.12293693103907422</v>
       </c>
       <c r="F36" s="3">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1">
-        <v>1</v>
+        <v>0.11</v>
+      </c>
+      <c r="G36" s="5">
+        <v>2</v>
       </c>
       <c r="H36" s="3">
-        <f>F36*G36</f>
-      </c>
-      <c r="I36" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J36" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="20.25">
+    <row r="37" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B37" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E37" s="3">
-        <v>0.9521987525747528</v>
+        <v>0.95219875257475284</v>
       </c>
       <c r="F37" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G37" s="1">
-        <v>1</v>
+        <v>0.11</v>
+      </c>
+      <c r="G37" s="5">
+        <v>2</v>
       </c>
       <c r="H37" s="3">
-        <f>F37*G37</f>
-      </c>
-      <c r="I37" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J37" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="20.25">
+    <row r="38" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="9" t="s">
         <v>63</v>
       </c>
       <c r="E38" s="3">
-        <v>0.642370787678666</v>
+        <v>0.64237078767866596</v>
       </c>
       <c r="F38" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1</v>
+        <v>0.11</v>
+      </c>
+      <c r="G38" s="5">
+        <v>2</v>
       </c>
       <c r="H38" s="3">
-        <f>F38*G38</f>
-      </c>
-      <c r="I38" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J38" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="20.25">
+    <row r="39" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>65</v>
       </c>
       <c r="E39" s="3">
-        <v>0.3123072636522166</v>
-      </c>
-      <c r="F39" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G39" s="1">
-        <v>4</v>
+        <v>0.31230726365221662</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G39" s="5">
+        <v>2</v>
       </c>
       <c r="H39" s="3">
-        <f>F39*G39</f>
-      </c>
-      <c r="I39" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J39" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="20.25">
+    <row r="40" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="9" t="s">
         <v>66</v>
       </c>
       <c r="E40" s="3">
         <v>0.29412414891305605</v>
       </c>
-      <c r="F40" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G40" s="1">
-        <v>4</v>
+      <c r="F40" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G40" s="5">
+        <v>2</v>
       </c>
       <c r="H40" s="3">
-        <f>F40*G40</f>
-      </c>
-      <c r="I40" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J40" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="20.25">
+    <row r="41" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="9" t="s">
         <v>67</v>
       </c>
       <c r="E41" s="3">
-        <v>0.4810439434160897</v>
-      </c>
-      <c r="F41" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G41" s="1">
+        <v>0.48104394341608969</v>
+      </c>
+      <c r="F41" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G41" s="5">
         <v>2</v>
       </c>
       <c r="H41" s="3">
-        <f>F41*G41</f>
-      </c>
-      <c r="I41" s="5"/>
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J41" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="20.25">
+    <row r="42" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="9" t="s">
         <v>68</v>
       </c>
       <c r="E42" s="3">
-        <v>0.6743343725835366</v>
-      </c>
-      <c r="F42" s="9">
-        <v>0.2</v>
-      </c>
-      <c r="G42" s="1">
-        <v>0</v>
+        <v>0.67433437258353657</v>
+      </c>
+      <c r="F42" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G42" s="5">
+        <v>2</v>
       </c>
       <c r="H42" s="1">
-        <f>F42*G42</f>
-      </c>
-      <c r="I42" s="5" t="s">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="I42" t="s">
         <v>23</v>
       </c>
       <c r="J42" s="3">
         <f>SUM(H34:H42)</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="20.25">
-      <c r="A43" s="6">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
         <v>42</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="9">
-        <v>0.3314614630361977</v>
+      <c r="E43" s="8">
+        <v>0.33146146303619772</v>
       </c>
       <c r="F43" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G43" s="6">
-        <v>1</v>
-      </c>
-      <c r="H43" s="9">
-        <f>F43*G43</f>
-      </c>
-      <c r="I43" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G43" s="5">
+        <v>2</v>
+      </c>
+      <c r="H43" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J43" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="20.25">
-      <c r="A44" s="6">
+    <row r="44" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
         <v>43</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E44" s="9">
-        <v>0.03598080991121799</v>
+      <c r="E44" s="8">
+        <v>3.5980809911217992E-2</v>
       </c>
       <c r="F44" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G44" s="6">
-        <v>2</v>
-      </c>
-      <c r="H44" s="9">
-        <f>F44*G44</f>
-      </c>
-      <c r="I44" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G44" s="5">
+        <v>2</v>
+      </c>
+      <c r="H44" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J44" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="20.25">
-      <c r="A45" s="6">
+    <row r="45" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
         <v>44</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E45" s="9">
-        <v>0.6587832433295059</v>
-      </c>
-      <c r="F45" s="9">
-        <v>1</v>
-      </c>
-      <c r="G45" s="6">
-        <v>2</v>
-      </c>
-      <c r="H45" s="9">
-        <f>F45*G45</f>
-      </c>
-      <c r="I45" s="5"/>
+      <c r="E45" s="8">
+        <v>0.65878324332950589</v>
+      </c>
+      <c r="F45" s="3">
+        <v>0.11</v>
+      </c>
+      <c r="G45" s="5">
+        <v>2</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J45" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="20.25">
-      <c r="A46" s="6">
+    <row r="46" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
         <v>45</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E46" s="9">
-        <v>0.7449981286269592</v>
+      <c r="E46" s="8">
+        <v>0.74499812862695924</v>
       </c>
       <c r="F46" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G46" s="6">
-        <v>2</v>
-      </c>
-      <c r="H46" s="9">
-        <f>F46*G46</f>
-      </c>
-      <c r="I46" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G46" s="5">
+        <v>2</v>
+      </c>
+      <c r="H46" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J46" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="20.25">
-      <c r="A47" s="6">
+    <row r="47" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
         <v>46</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="8">
         <v>0.23777100145271024</v>
       </c>
       <c r="F47" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G47" s="6">
-        <v>4</v>
-      </c>
-      <c r="H47" s="9">
-        <f>F47*G47</f>
-      </c>
-      <c r="I47" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G47" s="5">
+        <v>2</v>
+      </c>
+      <c r="H47" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J47" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="20.25">
-      <c r="A48" s="6">
+    <row r="48" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
         <v>47</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="9">
-        <v>0.7460047460721294</v>
+      <c r="E48" s="8">
+        <v>0.74600474607212941</v>
       </c>
       <c r="F48" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G48" s="6">
-        <v>1</v>
-      </c>
-      <c r="H48" s="9">
-        <f>F48*G48</f>
-      </c>
-      <c r="I48" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G48" s="5">
+        <v>2</v>
+      </c>
+      <c r="H48" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J48" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="20.25">
-      <c r="A49" s="6">
+    <row r="49" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
         <v>48</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="E49" s="9">
+      <c r="E49" s="8">
         <v>0.11599250894447277</v>
       </c>
       <c r="F49" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G49" s="6">
-        <v>1</v>
-      </c>
-      <c r="H49" s="9">
-        <f>F49*G49</f>
-      </c>
-      <c r="I49" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G49" s="5">
+        <v>2</v>
+      </c>
+      <c r="H49" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J49" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="20.25">
-      <c r="A50" s="6">
+    <row r="50" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
         <v>49</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="9">
-        <v>0.6406476871314409</v>
+      <c r="E50" s="8">
+        <v>0.64064768713144093</v>
       </c>
       <c r="F50" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G50" s="6">
-        <v>1</v>
-      </c>
-      <c r="H50" s="9">
-        <f>F50*G50</f>
-      </c>
-      <c r="I50" s="5"/>
+        <v>0.11</v>
+      </c>
+      <c r="G50" s="5">
+        <v>2</v>
+      </c>
+      <c r="H50" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
       <c r="J50" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="20.25">
-      <c r="A51" s="6">
+    <row r="51" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
         <v>50</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E51" s="9">
-        <v>0.6183831338624901</v>
+      <c r="E51" s="8">
+        <v>0.61838313386249011</v>
       </c>
       <c r="F51" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G51" s="6">
-        <v>3</v>
-      </c>
-      <c r="H51" s="9">
-        <f>F51*G51</f>
-      </c>
-      <c r="I51" s="5" t="s">
+        <v>0.11</v>
+      </c>
+      <c r="G51" s="5">
+        <v>2</v>
+      </c>
+      <c r="H51" s="8">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="I51" t="s">
         <v>23</v>
       </c>
       <c r="J51" s="3">
         <f>SUM(H43:H51)</f>
+        <v>1.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>